<commit_message>
- continue analyst shoppe.
</commit_message>
<xml_diff>
--- a/01. Description code in course.xlsx
+++ b/01. Description code in course.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\My Drive\02. Coursera\04.IBM_Generative_A_ Engineering_Professional_Certificate\07.Python_in_data_analyst\IBM_Python_in_data_analyst\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BBCA2C5-E6BB-472A-B3CC-1CA8FED2E0E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EAF482AF-DF16-4F0A-9A48-7B332C3B702E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7065" yWindow="2760" windowWidth="15420" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="21465" yWindow="1980" windowWidth="15420" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -936,8 +936,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A33" workbookViewId="0">
-      <selection activeCell="B40" sqref="B40"/>
+    <sheetView tabSelected="1" topLeftCell="A45" workbookViewId="0">
+      <selection activeCell="A49" sqref="A49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>

<commit_message>
-practice clean dataframe autos - use dropna() - use linspace() - use isnull() - use pd.cut() - use pd.get_dummies()
</commit_message>
<xml_diff>
--- a/01. Description code in course.xlsx
+++ b/01. Description code in course.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\My Drive\02. Coursera\04.IBM_Generative_A_ Engineering_Professional_Certificate\07.Python_in_data_analyst\IBM_Python_in_data_analyst\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EAF482AF-DF16-4F0A-9A48-7B332C3B702E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{252649AE-A9E5-42EF-B8ED-09A558BE420A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="21465" yWindow="1980" windowWidth="15420" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="11700" yWindow="1905" windowWidth="14325" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -183,12 +183,37 @@
         </r>
       </text>
     </comment>
+    <comment ref="C50" authorId="1" shapeId="0" xr:uid="{9BE8E2C5-1F48-48F8-900D-36262AF73386}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Admin:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+mean = df["normalize=losses"].mean()
+df["normalize-losses"].replace(np.nan, mean)</t>
+        </r>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="128">
   <si>
     <t>Pandas</t>
   </si>
@@ -566,6 +591,12 @@
   </si>
   <si>
     <t>the index parameter in the to_csv method controls whether the row index of the dataframe is written to the output CSV file</t>
+  </si>
+  <si>
+    <t>men()</t>
+  </si>
+  <si>
+    <t>calculation mean value in object</t>
   </si>
 </sst>
 </file>
@@ -934,10 +965,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G49"/>
+  <dimension ref="A1:G50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A45" workbookViewId="0">
-      <selection activeCell="A49" sqref="A49"/>
+    <sheetView tabSelected="1" topLeftCell="B45" workbookViewId="0">
+      <selection activeCell="C50" sqref="C50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1540,6 +1571,17 @@
         <v>125</v>
       </c>
     </row>
+    <row r="50" spans="1:3">
+      <c r="A50" t="s">
+        <v>83</v>
+      </c>
+      <c r="B50" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="C50" s="3" t="s">
+        <v>127</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>